<commit_message>
change code create groups Whatsapp
</commit_message>
<xml_diff>
--- a/EXCEL_TRABAJADO/2023-1.xlsx
+++ b/EXCEL_TRABAJADO/2023-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gians\Desktop\dev\UNDC_AUTOMATIZACION\EXCEL_TRABAJADO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E66C8C-9F01-431E-8E4A-FD625EF07FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9ABB28-CBF5-47A8-A26C-3361BE9066AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="885" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="1155" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="305">
   <si>
     <t>N°</t>
   </si>
@@ -890,6 +890,54 @@
   </si>
   <si>
     <t>https://aula.undc.edu.pe/course/view.php?id=309</t>
+  </si>
+  <si>
+    <t>AG63 - 583 - PROPAGACIÓN DE PLANTAS - 3253</t>
+  </si>
+  <si>
+    <t>MATOS LIZANA JULIO CESAR</t>
+  </si>
+  <si>
+    <t>AG64 - 584 - ENTOMOLOGÍA GENERAL - 3254</t>
+  </si>
+  <si>
+    <t>AG65 - 585 - TOPOGRAFÍA - 3255</t>
+  </si>
+  <si>
+    <t>EG20 - 586 - PENSAMIENTO POLÍTICO CONTEMPORÁNEO - 3256</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>CUELLAR FERNANDEZ JOSÉ MARTÍN</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/course/view.php?id=377</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/course/view.php?id=376</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/course/view.php?id=375</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/course/view.php?id=374</t>
+  </si>
+  <si>
+    <t>https://chat.whatsapp.com/Cr1yxFxmtbh9AUbrpyQXE6</t>
+  </si>
+  <si>
+    <t>https://chat.whatsapp.com/FPRS7x1liP3FfsFWvRgqfm</t>
+  </si>
+  <si>
+    <t>https://chat.whatsapp.com/Dt16YoLNiQSJ7ZWVznbNDr</t>
+  </si>
+  <si>
+    <t>https://chat.whatsapp.com/EaPviu0x5zLK02gHWUMznj</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1087,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1072,7 +1120,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
@@ -1379,11 +1426,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:AE65"/>
+  <dimension ref="A1:AE69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3140,76 +3187,76 @@
       <c r="AC23" s="10"/>
       <c r="AE23" s="8"/>
     </row>
-    <row r="24" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="16" t="s">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="16" t="s">
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24">
         <v>35</v>
       </c>
-      <c r="I24" s="16" t="s">
+      <c r="I24" t="s">
         <v>238</v>
       </c>
-      <c r="M24" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="S24" s="17" t="s">
+      <c r="M24" t="s">
+        <v>21</v>
+      </c>
+      <c r="S24" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="T24" s="16" t="s">
+      <c r="T24" t="s">
         <v>30</v>
       </c>
-      <c r="U24" s="18" t="s">
+      <c r="U24" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="V24" s="16" t="str">
+      <c r="V24" t="str">
         <f t="shared" si="3"/>
         <v>296</v>
       </c>
-      <c r="W24" s="16" t="str">
+      <c r="W24" t="str">
         <f t="shared" si="4"/>
         <v>FG.4 - 693</v>
       </c>
-      <c r="X24" s="16" t="str">
+      <c r="X24" t="str">
         <f t="shared" si="5"/>
         <v>LIDERAZGO Y EMPRENDIMIENTO - 3187</v>
       </c>
-      <c r="Y24" s="16" t="str">
+      <c r="Y24" t="str">
         <f t="shared" si="6"/>
         <v>AGRONOMIA III-M-A LIDERAZGO Y EMPRENDIMIENTO</v>
       </c>
-      <c r="Z24" s="16" t="str">
+      <c r="Z24" t="str">
         <f t="shared" si="7"/>
         <v>AG_III-M-A LIDERAZGO Y EMPRENDIMIENTO - 3187</v>
       </c>
-      <c r="AA24" s="16" t="str">
+      <c r="AA24" t="str">
         <f t="shared" si="8"/>
         <v>AG_III-M-A LIDERAZGO Y EM</v>
       </c>
-      <c r="AB24" s="16" t="str">
+      <c r="AB24" t="str">
         <f>CONCATENATE("&lt;p&gt;&lt;a href='",S24,"' target='_blank'&gt;&lt;img src='",items!$B$1,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FyCtwY0JIulKVH9bPcFmdq' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AC24" s="17"/>
-      <c r="AE24" s="18"/>
+      <c r="AC24" s="16"/>
+      <c r="AE24" s="17"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -6281,6 +6328,270 @@
       </c>
       <c r="AC65" s="10"/>
       <c r="AE65" s="8"/>
+    </row>
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" t="s">
+        <v>289</v>
+      </c>
+      <c r="E66" t="s">
+        <v>114</v>
+      </c>
+      <c r="F66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" t="s">
+        <v>20</v>
+      </c>
+      <c r="H66">
+        <v>9</v>
+      </c>
+      <c r="I66" t="s">
+        <v>290</v>
+      </c>
+      <c r="S66" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="T66" t="s">
+        <v>296</v>
+      </c>
+      <c r="U66" t="s">
+        <v>297</v>
+      </c>
+      <c r="V66" t="str">
+        <f t="shared" ref="V66:V69" si="9">MID(U66,45,4)</f>
+        <v>377</v>
+      </c>
+      <c r="W66" t="str">
+        <f t="shared" ref="W66:W69" si="10">MID(D66,1,10)</f>
+        <v>AG63 - 583</v>
+      </c>
+      <c r="X66" t="str">
+        <f t="shared" ref="X66:X69" si="11">TRIM(MID(D66,14,222))</f>
+        <v>PROPAGACIÓN DE PLANTAS - 3253</v>
+      </c>
+      <c r="Y66" t="str">
+        <f t="shared" ref="Y66:Y69" si="12">TRIM(CONCATENATE("AGRONOMIA ",E66,"-",F66,"-",G66," ",LEFT(X66,LEN(X66)-7)))</f>
+        <v>AGRONOMIA VI-M-A PROPAGACIÓN DE PLANTAS</v>
+      </c>
+      <c r="Z66" t="str">
+        <f t="shared" ref="Z66:Z69" si="13">CONCATENATE(B66,"_",E66,"-",F66,"-",G66," ",X66)</f>
+        <v>AG_VI-M-A PROPAGACIÓN DE PLANTAS - 3253</v>
+      </c>
+      <c r="AA66" t="str">
+        <f t="shared" ref="AA66:AA69" si="14">TRIM(MID(Z66,1,25))</f>
+        <v>AG_VI-M-A PROPAGACIÓN DE</v>
+      </c>
+      <c r="AB66" t="str">
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S66,"' target='_blank'&gt;&lt;img src='",items!$B$1,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Cr1yxFxmtbh9AUbrpyQXE6' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" t="s">
+        <v>291</v>
+      </c>
+      <c r="E67" t="s">
+        <v>114</v>
+      </c>
+      <c r="F67" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" t="s">
+        <v>20</v>
+      </c>
+      <c r="H67">
+        <v>2</v>
+      </c>
+      <c r="I67" t="s">
+        <v>290</v>
+      </c>
+      <c r="S67" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="T67" t="s">
+        <v>296</v>
+      </c>
+      <c r="U67" t="s">
+        <v>298</v>
+      </c>
+      <c r="V67" t="str">
+        <f t="shared" si="9"/>
+        <v>376</v>
+      </c>
+      <c r="W67" t="str">
+        <f t="shared" si="10"/>
+        <v>AG64 - 584</v>
+      </c>
+      <c r="X67" t="str">
+        <f t="shared" si="11"/>
+        <v>ENTOMOLOGÍA GENERAL - 3254</v>
+      </c>
+      <c r="Y67" t="str">
+        <f t="shared" si="12"/>
+        <v>AGRONOMIA VI-M-A ENTOMOLOGÍA GENERAL</v>
+      </c>
+      <c r="Z67" t="str">
+        <f t="shared" si="13"/>
+        <v>AG_VI-M-A ENTOMOLOGÍA GENERAL - 3254</v>
+      </c>
+      <c r="AA67" t="str">
+        <f t="shared" si="14"/>
+        <v>AG_VI-M-A ENTOMOLOGÍA GEN</v>
+      </c>
+      <c r="AB67" t="str">
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S67,"' target='_blank'&gt;&lt;img src='",items!$B$1,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FPRS7x1liP3FfsFWvRgqfm' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" t="s">
+        <v>292</v>
+      </c>
+      <c r="E68" t="s">
+        <v>114</v>
+      </c>
+      <c r="F68" t="s">
+        <v>18</v>
+      </c>
+      <c r="G68" t="s">
+        <v>20</v>
+      </c>
+      <c r="H68">
+        <v>26</v>
+      </c>
+      <c r="I68" t="s">
+        <v>290</v>
+      </c>
+      <c r="S68" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="T68" t="s">
+        <v>296</v>
+      </c>
+      <c r="U68" t="s">
+        <v>299</v>
+      </c>
+      <c r="V68" t="str">
+        <f t="shared" si="9"/>
+        <v>375</v>
+      </c>
+      <c r="W68" t="str">
+        <f t="shared" si="10"/>
+        <v>AG65 - 585</v>
+      </c>
+      <c r="X68" t="str">
+        <f t="shared" si="11"/>
+        <v>TOPOGRAFÍA - 3255</v>
+      </c>
+      <c r="Y68" t="str">
+        <f t="shared" si="12"/>
+        <v>AGRONOMIA VI-M-A TOPOGRAFÍA</v>
+      </c>
+      <c r="Z68" t="str">
+        <f t="shared" si="13"/>
+        <v>AG_VI-M-A TOPOGRAFÍA - 3255</v>
+      </c>
+      <c r="AA68" t="str">
+        <f t="shared" si="14"/>
+        <v>AG_VI-M-A TOPOGRAFÍA - 32</v>
+      </c>
+      <c r="AB68" t="str">
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S68,"' target='_blank'&gt;&lt;img src='",items!$B$1,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Dt16YoLNiQSJ7ZWVznbNDr' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" t="s">
+        <v>293</v>
+      </c>
+      <c r="E69" t="s">
+        <v>114</v>
+      </c>
+      <c r="F69" t="s">
+        <v>294</v>
+      </c>
+      <c r="G69" t="s">
+        <v>20</v>
+      </c>
+      <c r="H69">
+        <v>7</v>
+      </c>
+      <c r="I69" t="s">
+        <v>295</v>
+      </c>
+      <c r="S69" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="T69" t="s">
+        <v>296</v>
+      </c>
+      <c r="U69" t="s">
+        <v>300</v>
+      </c>
+      <c r="V69" t="str">
+        <f t="shared" si="9"/>
+        <v>374</v>
+      </c>
+      <c r="W69" t="str">
+        <f t="shared" si="10"/>
+        <v>EG20 - 586</v>
+      </c>
+      <c r="X69" t="str">
+        <f t="shared" si="11"/>
+        <v>PENSAMIENTO POLÍTICO CONTEMPORÁNEO - 3256</v>
+      </c>
+      <c r="Y69" t="str">
+        <f t="shared" si="12"/>
+        <v>AGRONOMIA VI-N-A PENSAMIENTO POLÍTICO CONTEMPORÁNEO</v>
+      </c>
+      <c r="Z69" t="str">
+        <f t="shared" si="13"/>
+        <v>AG_VI-N-A PENSAMIENTO POLÍTICO CONTEMPORÁNEO - 3256</v>
+      </c>
+      <c r="AA69" t="str">
+        <f t="shared" si="14"/>
+        <v>AG_VI-N-A PENSAMIENTO POL</v>
+      </c>
+      <c r="AB69" t="str">
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S69,"' target='_blank'&gt;&lt;img src='",items!$B$1,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/EaPviu0x5zLK02gHWUMznj' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -6346,9 +6657,13 @@
     <hyperlink ref="S64" r:id="rId59" xr:uid="{7BD1F2A1-59AA-4400-869E-BA5A3BE9EDA2}"/>
     <hyperlink ref="S65" r:id="rId60" xr:uid="{3D148C96-95BF-485D-A696-031D5F013451}"/>
     <hyperlink ref="U43" r:id="rId61" xr:uid="{17D1D465-4044-49FA-99D7-656B84B8D63E}"/>
+    <hyperlink ref="S66" r:id="rId62" xr:uid="{0C90488E-CCF0-4D03-A583-B535D2B6CCCB}"/>
+    <hyperlink ref="S67" r:id="rId63" xr:uid="{0DD32316-3FFE-4604-9BD6-351053D73B0E}"/>
+    <hyperlink ref="S68" r:id="rId64" xr:uid="{144D8471-20D0-4D2C-802C-95648339E2A1}"/>
+    <hyperlink ref="S69" r:id="rId65" xr:uid="{E7E3DF2C-10C4-4306-B67C-BBFD53E54BFC}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId62"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId66"/>
 </worksheet>
 </file>
 
@@ -8718,7 +9033,7 @@
       </c>
       <c r="B9">
         <f>COUNTIFS(Sheet!E:E,items!A9)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -8760,7 +9075,7 @@
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14">
         <f>SUM(B4:B13)</f>
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Envio de mensajes Whatsapp
</commit_message>
<xml_diff>
--- a/EXCEL_TRABAJADO/2023-1.xlsx
+++ b/EXCEL_TRABAJADO/2023-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gians\Desktop\dev\UNDC_AUTOMATIZACION\EXCEL_TRABAJADO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9ABB28-CBF5-47A8-A26C-3361BE9066AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA643CCD-2D02-4F28-90F4-432A29505851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1155" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="308">
   <si>
     <t>N°</t>
   </si>
@@ -938,6 +938,15 @@
   </si>
   <si>
     <t>https://chat.whatsapp.com/EaPviu0x5zLK02gHWUMznj</t>
+  </si>
+  <si>
+    <t>AG76 - 592 - FITOPATOLOGÍA GENERAL - 3259</t>
+  </si>
+  <si>
+    <t>TARDE</t>
+  </si>
+  <si>
+    <t>https://chat.whatsapp.com/HCW8kplTG7DHTjzNrQJlKW</t>
   </si>
 </sst>
 </file>
@@ -1426,11 +1435,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:AE69"/>
+  <dimension ref="A1:AE70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3372,7 +3381,7 @@
         <v>186</v>
       </c>
       <c r="T26" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U26" s="13" t="s">
         <v>146</v>
@@ -3451,7 +3460,7 @@
         <v>187</v>
       </c>
       <c r="T27" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U27" s="13" t="s">
         <v>149</v>
@@ -3530,7 +3539,7 @@
         <v>188</v>
       </c>
       <c r="T28" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U28" s="13" t="s">
         <v>139</v>
@@ -3609,7 +3618,7 @@
         <v>189</v>
       </c>
       <c r="T29" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U29" s="13" t="s">
         <v>152</v>
@@ -3688,7 +3697,7 @@
         <v>190</v>
       </c>
       <c r="T30" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U30" s="13" t="s">
         <v>141</v>
@@ -3767,7 +3776,7 @@
         <v>191</v>
       </c>
       <c r="T31" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U31" s="13" t="s">
         <v>153</v>
@@ -3846,7 +3855,7 @@
         <v>192</v>
       </c>
       <c r="T32" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U32" s="13" t="s">
         <v>148</v>
@@ -3925,7 +3934,7 @@
         <v>193</v>
       </c>
       <c r="T33" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U33" s="13" t="s">
         <v>155</v>
@@ -4004,7 +4013,7 @@
         <v>194</v>
       </c>
       <c r="T34" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U34" s="13" t="s">
         <v>143</v>
@@ -4083,7 +4092,7 @@
         <v>195</v>
       </c>
       <c r="T35" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U35" s="13" t="s">
         <v>150</v>
@@ -4162,7 +4171,7 @@
         <v>196</v>
       </c>
       <c r="T36" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U36" s="13" t="s">
         <v>145</v>
@@ -4241,7 +4250,7 @@
         <v>197</v>
       </c>
       <c r="T37" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U37" s="13" t="s">
         <v>151</v>
@@ -4320,7 +4329,7 @@
         <v>198</v>
       </c>
       <c r="T38" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U38" s="13" t="s">
         <v>147</v>
@@ -4399,7 +4408,7 @@
         <v>199</v>
       </c>
       <c r="T39" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U39" s="13" t="s">
         <v>154</v>
@@ -4470,7 +4479,7 @@
         <v>200</v>
       </c>
       <c r="T40" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U40" t="s">
         <v>279</v>
@@ -4541,7 +4550,7 @@
         <v>201</v>
       </c>
       <c r="T41" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U41" t="s">
         <v>280</v>
@@ -4612,7 +4621,7 @@
         <v>202</v>
       </c>
       <c r="T42" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U42" t="s">
         <v>281</v>
@@ -4683,7 +4692,7 @@
         <v>203</v>
       </c>
       <c r="T43" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U43" s="8" t="s">
         <v>282</v>
@@ -4754,7 +4763,7 @@
         <v>204</v>
       </c>
       <c r="T44" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U44" t="s">
         <v>283</v>
@@ -4825,7 +4834,7 @@
         <v>205</v>
       </c>
       <c r="T45" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U45" t="s">
         <v>128</v>
@@ -4896,7 +4905,7 @@
         <v>206</v>
       </c>
       <c r="T46" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U46" t="s">
         <v>284</v>
@@ -4967,7 +4976,7 @@
         <v>207</v>
       </c>
       <c r="T47" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U47" s="8" t="s">
         <v>130</v>
@@ -5038,7 +5047,7 @@
         <v>208</v>
       </c>
       <c r="T48" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U48" t="s">
         <v>285</v>
@@ -5109,7 +5118,7 @@
         <v>209</v>
       </c>
       <c r="T49" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U49" t="s">
         <v>126</v>
@@ -5180,7 +5189,7 @@
         <v>210</v>
       </c>
       <c r="T50" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U50" t="s">
         <v>286</v>
@@ -5251,7 +5260,7 @@
         <v>211</v>
       </c>
       <c r="T51" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U51" t="s">
         <v>287</v>
@@ -5322,7 +5331,7 @@
         <v>212</v>
       </c>
       <c r="T52" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U52" t="s">
         <v>288</v>
@@ -5393,7 +5402,7 @@
         <v>213</v>
       </c>
       <c r="T53" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U53" t="s">
         <v>134</v>
@@ -5472,7 +5481,7 @@
         <v>214</v>
       </c>
       <c r="T54" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U54" s="13" t="s">
         <v>132</v>
@@ -5551,7 +5560,7 @@
         <v>215</v>
       </c>
       <c r="T55" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U55" s="13" t="s">
         <v>129</v>
@@ -5630,7 +5639,7 @@
         <v>216</v>
       </c>
       <c r="T56" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U56" s="13" t="s">
         <v>131</v>
@@ -5709,7 +5718,7 @@
         <v>217</v>
       </c>
       <c r="T57" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U57" s="13" t="s">
         <v>127</v>
@@ -5788,7 +5797,7 @@
         <v>218</v>
       </c>
       <c r="T58" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U58" s="13" t="s">
         <v>135</v>
@@ -5867,7 +5876,7 @@
         <v>219</v>
       </c>
       <c r="T59" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U59" s="13" t="s">
         <v>136</v>
@@ -5938,7 +5947,7 @@
         <v>220</v>
       </c>
       <c r="T60" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U60" t="s">
         <v>137</v>
@@ -6009,7 +6018,7 @@
         <v>221</v>
       </c>
       <c r="T61" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U61" t="s">
         <v>133</v>
@@ -6080,7 +6089,7 @@
         <v>222</v>
       </c>
       <c r="T62" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U62" t="s">
         <v>142</v>
@@ -6151,7 +6160,7 @@
         <v>223</v>
       </c>
       <c r="T63" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U63" t="s">
         <v>144</v>
@@ -6222,7 +6231,7 @@
         <v>224</v>
       </c>
       <c r="T64" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U64" t="s">
         <v>138</v>
@@ -6293,7 +6302,7 @@
         <v>225</v>
       </c>
       <c r="T65" t="s">
-        <v>30</v>
+        <v>296</v>
       </c>
       <c r="U65" t="s">
         <v>140</v>
@@ -6591,6 +6600,72 @@
       <c r="AB69" t="str">
         <f>CONCATENATE("&lt;p&gt;&lt;a href='",S69,"' target='_blank'&gt;&lt;img src='",items!$B$1,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/EaPviu0x5zLK02gHWUMznj' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>77</v>
+      </c>
+      <c r="B70" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" t="s">
+        <v>305</v>
+      </c>
+      <c r="E70" t="s">
+        <v>27</v>
+      </c>
+      <c r="F70" t="s">
+        <v>306</v>
+      </c>
+      <c r="G70" t="s">
+        <v>23</v>
+      </c>
+      <c r="H70">
+        <v>20</v>
+      </c>
+      <c r="I70" t="s">
+        <v>254</v>
+      </c>
+      <c r="S70" t="s">
+        <v>307</v>
+      </c>
+      <c r="T70" t="s">
+        <v>296</v>
+      </c>
+      <c r="U70" t="s">
+        <v>299</v>
+      </c>
+      <c r="V70" t="str">
+        <f t="shared" ref="V70" si="15">MID(U70,45,4)</f>
+        <v>375</v>
+      </c>
+      <c r="W70" t="str">
+        <f t="shared" ref="W70" si="16">MID(D70,1,10)</f>
+        <v>AG76 - 592</v>
+      </c>
+      <c r="X70" t="str">
+        <f t="shared" ref="X70" si="17">TRIM(MID(D70,14,222))</f>
+        <v>FITOPATOLOGÍA GENERAL - 3259</v>
+      </c>
+      <c r="Y70" t="str">
+        <f t="shared" ref="Y70" si="18">TRIM(CONCATENATE("AGRONOMIA ",E70,"-",F70,"-",G70," ",LEFT(X70,LEN(X70)-7)))</f>
+        <v>AGRONOMIA VII-TARDE-B FITOPATOLOGÍA GENERAL</v>
+      </c>
+      <c r="Z70" t="str">
+        <f t="shared" ref="Z70" si="19">CONCATENATE(B70,"_",E70,"-",F70,"-",G70," ",X70)</f>
+        <v>AG_VII-TARDE-B FITOPATOLOGÍA GENERAL - 3259</v>
+      </c>
+      <c r="AA70" t="str">
+        <f t="shared" ref="AA70" si="20">TRIM(MID(Z70,1,25))</f>
+        <v>AG_VII-TARDE-B FITOPATOLO</v>
+      </c>
+      <c r="AB70" t="str">
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S70,"' target='_blank'&gt;&lt;img src='",items!$B$1,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/HCW8kplTG7DHTjzNrQJlKW' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
     </row>
   </sheetData>
@@ -9042,7 +9117,7 @@
       </c>
       <c r="B10">
         <f>COUNTIFS(Sheet!E:E,items!A10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -9075,7 +9150,7 @@
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14">
         <f>SUM(B4:B13)</f>
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Nueva actualizacion del driverchrome
</commit_message>
<xml_diff>
--- a/EXCEL_TRABAJADO/2023-1.xlsx
+++ b/EXCEL_TRABAJADO/2023-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gians\Desktop\dev\UNDC_AUTOMATIZACION\EXCEL_TRABAJADO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED602AF-C189-4881-96C2-9EB6564391C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76B88DD-D144-4192-9EFA-3906B83BFA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="308">
   <si>
     <t>N°</t>
   </si>
@@ -944,13 +944,16 @@
   </si>
   <si>
     <t>https://chat.whatsapp.com/HCW8kplTG7DHTjzNrQJlKW</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1434,12 +1437,12 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AE70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W17" sqref="W17"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA67" sqref="AA67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
@@ -1465,7 +1468,7 @@
     <col min="31" max="31" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="29.25" customHeight="1">
+    <row r="1" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1535,7 +1538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1578,7 +1581,7 @@
         <v>161</v>
       </c>
       <c r="T2" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U2" s="14" t="s">
         <v>254</v>
@@ -1614,7 +1617,7 @@
       <c r="AC2" s="10"/>
       <c r="AE2" s="8"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>162</v>
       </c>
       <c r="T3" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U3" s="13" t="s">
         <v>255</v>
@@ -1683,7 +1686,7 @@
         <v>AG_I-T-B INTRODUCCIÓN A LA AGRONOMÍA - 3178</v>
       </c>
       <c r="AA3" t="str">
-        <f t="shared" ref="AA3:AA65" si="8">TRIM(MID(Z3,1,25))</f>
+        <f t="shared" ref="AA3:AA66" si="8">TRIM(MID(Z3,1,25))</f>
         <v>AG_I-T-B INTRODUCCIÓN A L</v>
       </c>
       <c r="AB3" t="str">
@@ -1693,7 +1696,7 @@
       <c r="AC3" s="10"/>
       <c r="AE3" s="8"/>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1736,7 +1739,7 @@
         <v>163</v>
       </c>
       <c r="T4" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U4" s="13" t="s">
         <v>256</v>
@@ -1772,7 +1775,7 @@
       <c r="AC4" s="10"/>
       <c r="AE4" s="8"/>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>164</v>
       </c>
       <c r="T5" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U5" s="13" t="s">
         <v>257</v>
@@ -1851,7 +1854,7 @@
       <c r="AC5" s="10"/>
       <c r="AE5" s="8"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -1894,7 +1897,7 @@
         <v>165</v>
       </c>
       <c r="T6" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U6" s="13" t="s">
         <v>258</v>
@@ -1930,7 +1933,7 @@
       <c r="AC6" s="10"/>
       <c r="AE6" s="8"/>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -1973,7 +1976,7 @@
         <v>166</v>
       </c>
       <c r="T7" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U7" s="14" t="s">
         <v>259</v>
@@ -2009,7 +2012,7 @@
       <c r="AC7" s="10"/>
       <c r="AE7" s="8"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -2052,7 +2055,7 @@
         <v>167</v>
       </c>
       <c r="T8" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U8" s="13" t="s">
         <v>260</v>
@@ -2088,7 +2091,7 @@
       <c r="AC8" s="10"/>
       <c r="AE8" s="8"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -2131,7 +2134,7 @@
         <v>168</v>
       </c>
       <c r="T9" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U9" s="13" t="s">
         <v>261</v>
@@ -2167,7 +2170,7 @@
       <c r="AC9" s="10"/>
       <c r="AE9" s="8"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -2210,7 +2213,7 @@
         <v>169</v>
       </c>
       <c r="T10" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U10" s="13" t="s">
         <v>262</v>
@@ -2246,7 +2249,7 @@
       <c r="AC10" s="10"/>
       <c r="AE10" s="8"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -2289,7 +2292,7 @@
         <v>170</v>
       </c>
       <c r="T11" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U11" s="14" t="s">
         <v>263</v>
@@ -2325,7 +2328,7 @@
       <c r="AC11" s="10"/>
       <c r="AE11" s="8"/>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>11</v>
       </c>
@@ -2368,7 +2371,7 @@
         <v>171</v>
       </c>
       <c r="T12" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U12" s="13" t="s">
         <v>264</v>
@@ -2404,7 +2407,7 @@
       <c r="AC12" s="10"/>
       <c r="AE12" s="8"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>12</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>172</v>
       </c>
       <c r="T13" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U13" s="13" t="s">
         <v>265</v>
@@ -2483,7 +2486,7 @@
       <c r="AC13" s="10"/>
       <c r="AE13" s="8"/>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2518,7 +2521,7 @@
         <v>173</v>
       </c>
       <c r="T14" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U14" t="s">
         <v>266</v>
@@ -2554,7 +2557,7 @@
       <c r="AC14" s="10"/>
       <c r="AE14" s="8"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>174</v>
       </c>
       <c r="T15" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U15" t="s">
         <v>267</v>
@@ -2625,7 +2628,7 @@
       <c r="AC15" s="10"/>
       <c r="AE15" s="8"/>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2660,7 +2663,7 @@
         <v>175</v>
       </c>
       <c r="T16" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U16" t="s">
         <v>268</v>
@@ -2696,7 +2699,7 @@
       <c r="AC16" s="10"/>
       <c r="AE16" s="8"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2731,7 +2734,7 @@
         <v>176</v>
       </c>
       <c r="T17" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U17" t="s">
         <v>269</v>
@@ -2767,7 +2770,7 @@
       <c r="AC17" s="10"/>
       <c r="AE17" s="8"/>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2802,7 +2805,7 @@
         <v>177</v>
       </c>
       <c r="T18" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U18" t="s">
         <v>270</v>
@@ -2838,7 +2841,7 @@
       <c r="AC18" s="10"/>
       <c r="AE18" s="8"/>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2873,7 +2876,7 @@
         <v>178</v>
       </c>
       <c r="T19" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U19" t="s">
         <v>271</v>
@@ -2909,7 +2912,7 @@
       <c r="AC19" s="10"/>
       <c r="AE19" s="8"/>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2944,7 +2947,7 @@
         <v>179</v>
       </c>
       <c r="T20" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U20" t="s">
         <v>272</v>
@@ -2980,7 +2983,7 @@
       <c r="AC20" s="10"/>
       <c r="AE20" s="8"/>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3015,7 +3018,7 @@
         <v>180</v>
       </c>
       <c r="T21" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U21" t="s">
         <v>273</v>
@@ -3051,7 +3054,7 @@
       <c r="AC21" s="10"/>
       <c r="AE21" s="8"/>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3086,7 +3089,7 @@
         <v>181</v>
       </c>
       <c r="T22" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U22" t="s">
         <v>274</v>
@@ -3122,7 +3125,7 @@
       <c r="AC22" s="10"/>
       <c r="AE22" s="8"/>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3157,7 +3160,7 @@
         <v>182</v>
       </c>
       <c r="T23" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U23" t="s">
         <v>275</v>
@@ -3193,7 +3196,7 @@
       <c r="AC23" s="10"/>
       <c r="AE23" s="8"/>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3228,7 +3231,7 @@
         <v>183</v>
       </c>
       <c r="T24" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U24" s="17" t="s">
         <v>276</v>
@@ -3264,7 +3267,7 @@
       <c r="AC24" s="16"/>
       <c r="AE24" s="17"/>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3299,7 +3302,7 @@
         <v>184</v>
       </c>
       <c r="T25" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U25" t="s">
         <v>277</v>
@@ -3335,7 +3338,7 @@
       <c r="AC25" s="10"/>
       <c r="AE25" s="8"/>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>25</v>
       </c>
@@ -3378,7 +3381,7 @@
         <v>185</v>
       </c>
       <c r="T26" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U26" s="13" t="s">
         <v>145</v>
@@ -3414,7 +3417,7 @@
       <c r="AC26" s="10"/>
       <c r="AE26" s="8"/>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>26</v>
       </c>
@@ -3457,7 +3460,7 @@
         <v>186</v>
       </c>
       <c r="T27" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U27" s="13" t="s">
         <v>148</v>
@@ -3493,7 +3496,7 @@
       <c r="AC27" s="10"/>
       <c r="AE27" s="8"/>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>27</v>
       </c>
@@ -3536,7 +3539,7 @@
         <v>187</v>
       </c>
       <c r="T28" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U28" s="13" t="s">
         <v>138</v>
@@ -3572,7 +3575,7 @@
       <c r="AC28" s="10"/>
       <c r="AE28" s="8"/>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>28</v>
       </c>
@@ -3615,7 +3618,7 @@
         <v>188</v>
       </c>
       <c r="T29" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U29" s="13" t="s">
         <v>151</v>
@@ -3651,7 +3654,7 @@
       <c r="AC29" s="10"/>
       <c r="AE29" s="8"/>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>29</v>
       </c>
@@ -3694,7 +3697,7 @@
         <v>189</v>
       </c>
       <c r="T30" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U30" s="13" t="s">
         <v>140</v>
@@ -3730,7 +3733,7 @@
       <c r="AC30" s="10"/>
       <c r="AE30" s="8"/>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>30</v>
       </c>
@@ -3773,7 +3776,7 @@
         <v>190</v>
       </c>
       <c r="T31" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U31" s="13" t="s">
         <v>152</v>
@@ -3809,7 +3812,7 @@
       <c r="AC31" s="10"/>
       <c r="AE31" s="8"/>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>31</v>
       </c>
@@ -3852,7 +3855,7 @@
         <v>191</v>
       </c>
       <c r="T32" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U32" s="13" t="s">
         <v>147</v>
@@ -3888,7 +3891,7 @@
       <c r="AC32" s="10"/>
       <c r="AE32" s="8"/>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>32</v>
       </c>
@@ -3931,7 +3934,7 @@
         <v>192</v>
       </c>
       <c r="T33" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U33" s="13" t="s">
         <v>154</v>
@@ -3967,7 +3970,7 @@
       <c r="AC33" s="10"/>
       <c r="AE33" s="8"/>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>33</v>
       </c>
@@ -4010,7 +4013,7 @@
         <v>193</v>
       </c>
       <c r="T34" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U34" s="13" t="s">
         <v>142</v>
@@ -4046,7 +4049,7 @@
       <c r="AC34" s="10"/>
       <c r="AE34" s="8"/>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>34</v>
       </c>
@@ -4089,7 +4092,7 @@
         <v>194</v>
       </c>
       <c r="T35" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U35" s="13" t="s">
         <v>149</v>
@@ -4125,7 +4128,7 @@
       <c r="AC35" s="10"/>
       <c r="AE35" s="8"/>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>35</v>
       </c>
@@ -4168,7 +4171,7 @@
         <v>195</v>
       </c>
       <c r="T36" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U36" s="13" t="s">
         <v>144</v>
@@ -4204,7 +4207,7 @@
       <c r="AC36" s="10"/>
       <c r="AE36" s="8"/>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>36</v>
       </c>
@@ -4247,7 +4250,7 @@
         <v>196</v>
       </c>
       <c r="T37" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U37" s="13" t="s">
         <v>150</v>
@@ -4283,7 +4286,7 @@
       <c r="AC37" s="10"/>
       <c r="AE37" s="8"/>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>37</v>
       </c>
@@ -4326,7 +4329,7 @@
         <v>197</v>
       </c>
       <c r="T38" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U38" s="13" t="s">
         <v>146</v>
@@ -4362,7 +4365,7 @@
       <c r="AC38" s="10"/>
       <c r="AE38" s="8"/>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>38</v>
       </c>
@@ -4405,7 +4408,7 @@
         <v>198</v>
       </c>
       <c r="T39" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U39" s="13" t="s">
         <v>153</v>
@@ -4441,7 +4444,7 @@
       <c r="AC39" s="10"/>
       <c r="AE39" s="8"/>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4476,7 +4479,7 @@
         <v>199</v>
       </c>
       <c r="T40" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U40" t="s">
         <v>278</v>
@@ -4512,7 +4515,7 @@
       <c r="AC40" s="10"/>
       <c r="AE40" s="8"/>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4547,7 +4550,7 @@
         <v>200</v>
       </c>
       <c r="T41" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U41" t="s">
         <v>279</v>
@@ -4583,7 +4586,7 @@
       <c r="AC41" s="10"/>
       <c r="AE41" s="8"/>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4618,7 +4621,7 @@
         <v>201</v>
       </c>
       <c r="T42" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U42" t="s">
         <v>280</v>
@@ -4654,7 +4657,7 @@
       <c r="AC42" s="10"/>
       <c r="AE42" s="8"/>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4689,7 +4692,7 @@
         <v>202</v>
       </c>
       <c r="T43" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U43" s="8" t="s">
         <v>281</v>
@@ -4725,7 +4728,7 @@
       <c r="AC43" s="10"/>
       <c r="AE43" s="8"/>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4760,7 +4763,7 @@
         <v>203</v>
       </c>
       <c r="T44" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U44" t="s">
         <v>282</v>
@@ -4796,7 +4799,7 @@
       <c r="AC44" s="10"/>
       <c r="AE44" s="8"/>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4831,7 +4834,7 @@
         <v>204</v>
       </c>
       <c r="T45" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U45" t="s">
         <v>127</v>
@@ -4867,7 +4870,7 @@
       <c r="AC45" s="10"/>
       <c r="AE45" s="8"/>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4902,7 +4905,7 @@
         <v>205</v>
       </c>
       <c r="T46" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U46" t="s">
         <v>283</v>
@@ -4938,7 +4941,7 @@
       <c r="AC46" s="10"/>
       <c r="AE46" s="8"/>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4973,7 +4976,7 @@
         <v>206</v>
       </c>
       <c r="T47" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U47" s="8" t="s">
         <v>129</v>
@@ -5009,7 +5012,7 @@
       <c r="AC47" s="10"/>
       <c r="AE47" s="8"/>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5044,7 +5047,7 @@
         <v>207</v>
       </c>
       <c r="T48" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U48" t="s">
         <v>284</v>
@@ -5080,7 +5083,7 @@
       <c r="AC48" s="10"/>
       <c r="AE48" s="8"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5115,7 +5118,7 @@
         <v>208</v>
       </c>
       <c r="T49" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U49" t="s">
         <v>125</v>
@@ -5151,7 +5154,7 @@
       <c r="AC49" s="10"/>
       <c r="AE49" s="8"/>
     </row>
-    <row r="50" spans="1:31">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5186,7 +5189,7 @@
         <v>209</v>
       </c>
       <c r="T50" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U50" t="s">
         <v>285</v>
@@ -5222,7 +5225,7 @@
       <c r="AC50" s="10"/>
       <c r="AE50" s="8"/>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5257,7 +5260,7 @@
         <v>210</v>
       </c>
       <c r="T51" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U51" t="s">
         <v>286</v>
@@ -5293,7 +5296,7 @@
       <c r="AC51" s="10"/>
       <c r="AE51" s="8"/>
     </row>
-    <row r="52" spans="1:31">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5328,7 +5331,7 @@
         <v>211</v>
       </c>
       <c r="T52" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U52" t="s">
         <v>287</v>
@@ -5364,7 +5367,7 @@
       <c r="AC52" s="10"/>
       <c r="AE52" s="8"/>
     </row>
-    <row r="53" spans="1:31">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5399,7 +5402,7 @@
         <v>212</v>
       </c>
       <c r="T53" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U53" t="s">
         <v>133</v>
@@ -5435,7 +5438,7 @@
       <c r="AC53" s="10"/>
       <c r="AE53" s="8"/>
     </row>
-    <row r="54" spans="1:31">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>53</v>
       </c>
@@ -5478,7 +5481,7 @@
         <v>213</v>
       </c>
       <c r="T54" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U54" s="13" t="s">
         <v>131</v>
@@ -5514,7 +5517,7 @@
       <c r="AC54" s="10"/>
       <c r="AE54" s="8"/>
     </row>
-    <row r="55" spans="1:31">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>54</v>
       </c>
@@ -5557,7 +5560,7 @@
         <v>214</v>
       </c>
       <c r="T55" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U55" s="13" t="s">
         <v>128</v>
@@ -5593,7 +5596,7 @@
       <c r="AC55" s="10"/>
       <c r="AE55" s="8"/>
     </row>
-    <row r="56" spans="1:31">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>55</v>
       </c>
@@ -5636,7 +5639,7 @@
         <v>215</v>
       </c>
       <c r="T56" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U56" s="13" t="s">
         <v>130</v>
@@ -5672,7 +5675,7 @@
       <c r="AC56" s="10"/>
       <c r="AE56" s="8"/>
     </row>
-    <row r="57" spans="1:31">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>56</v>
       </c>
@@ -5715,7 +5718,7 @@
         <v>216</v>
       </c>
       <c r="T57" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U57" s="13" t="s">
         <v>126</v>
@@ -5751,7 +5754,7 @@
       <c r="AC57" s="10"/>
       <c r="AE57" s="8"/>
     </row>
-    <row r="58" spans="1:31">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>57</v>
       </c>
@@ -5794,7 +5797,7 @@
         <v>217</v>
       </c>
       <c r="T58" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U58" s="13" t="s">
         <v>134</v>
@@ -5830,7 +5833,7 @@
       <c r="AC58" s="10"/>
       <c r="AE58" s="8"/>
     </row>
-    <row r="59" spans="1:31">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>58</v>
       </c>
@@ -5873,7 +5876,7 @@
         <v>218</v>
       </c>
       <c r="T59" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U59" s="13" t="s">
         <v>135</v>
@@ -5909,7 +5912,7 @@
       <c r="AC59" s="10"/>
       <c r="AE59" s="8"/>
     </row>
-    <row r="60" spans="1:31">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5944,7 +5947,7 @@
         <v>219</v>
       </c>
       <c r="T60" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U60" t="s">
         <v>136</v>
@@ -5980,7 +5983,7 @@
       <c r="AC60" s="10"/>
       <c r="AE60" s="8"/>
     </row>
-    <row r="61" spans="1:31">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -6015,7 +6018,7 @@
         <v>220</v>
       </c>
       <c r="T61" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U61" t="s">
         <v>132</v>
@@ -6051,7 +6054,7 @@
       <c r="AC61" s="10"/>
       <c r="AE61" s="8"/>
     </row>
-    <row r="62" spans="1:31">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6086,7 +6089,7 @@
         <v>221</v>
       </c>
       <c r="T62" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U62" t="s">
         <v>141</v>
@@ -6122,7 +6125,7 @@
       <c r="AC62" s="10"/>
       <c r="AE62" s="8"/>
     </row>
-    <row r="63" spans="1:31">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -6157,7 +6160,7 @@
         <v>222</v>
       </c>
       <c r="T63" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U63" t="s">
         <v>143</v>
@@ -6193,7 +6196,7 @@
       <c r="AC63" s="10"/>
       <c r="AE63" s="8"/>
     </row>
-    <row r="64" spans="1:31">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6228,7 +6231,7 @@
         <v>223</v>
       </c>
       <c r="T64" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U64" t="s">
         <v>137</v>
@@ -6264,7 +6267,7 @@
       <c r="AC64" s="10"/>
       <c r="AE64" s="8"/>
     </row>
-    <row r="65" spans="1:31">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6299,7 +6302,7 @@
         <v>224</v>
       </c>
       <c r="T65" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="U65" t="s">
         <v>139</v>
@@ -6335,7 +6338,7 @@
       <c r="AC65" s="10"/>
       <c r="AE65" s="8"/>
     </row>
-    <row r="66" spans="1:31">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -6393,7 +6396,7 @@
         <v>AG_VI-M-A PROPAGACIÓN DE PLANTAS - 3253</v>
       </c>
       <c r="AA66" t="str">
-        <f t="shared" ref="AA66:AA69" si="14">TRIM(MID(Z66,1,25))</f>
+        <f t="shared" si="8"/>
         <v>AG_VI-M-A PROPAGACIÓN DE</v>
       </c>
       <c r="AB66" t="str">
@@ -6401,7 +6404,7 @@
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Cr1yxFxmtbh9AUbrpyQXE6' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
     </row>
-    <row r="67" spans="1:31">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6459,7 +6462,7 @@
         <v>AG_VI-M-A ENTOMOLOGÍA GENERAL - 3254</v>
       </c>
       <c r="AA67" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="AA67:AA70" si="14">TRIM(MID(Z67,1,25))</f>
         <v>AG_VI-M-A ENTOMOLOGÍA GEN</v>
       </c>
       <c r="AB67" t="str">
@@ -6467,7 +6470,7 @@
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FPRS7x1liP3FfsFWvRgqfm' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
     </row>
-    <row r="68" spans="1:31">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>68</v>
       </c>
@@ -6533,7 +6536,7 @@
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Dt16YoLNiQSJ7ZWVznbNDr' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
     </row>
-    <row r="69" spans="1:31">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>70</v>
       </c>
@@ -6599,7 +6602,7 @@
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/EaPviu0x5zLK02gHWUMznj' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
     </row>
-    <row r="70" spans="1:31">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>77</v>
       </c>
@@ -6657,7 +6660,7 @@
         <v>AG_VII-TARDE-B FITOPATOLOGÍA GENERAL - 3259</v>
       </c>
       <c r="AA70" t="str">
-        <f t="shared" ref="AA70" si="20">TRIM(MID(Z70,1,25))</f>
+        <f t="shared" si="14"/>
         <v>AG_VII-TARDE-B FITOPATOLO</v>
       </c>
       <c r="AB70" t="str">
@@ -6747,7 +6750,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" bestFit="1" customWidth="1"/>
@@ -6760,7 +6763,7 @@
     <col min="9" max="9" width="40.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -6789,7 +6792,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -6821,7 +6824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -6853,7 +6856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -6885,7 +6888,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -6917,7 +6920,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -6949,7 +6952,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -6981,7 +6984,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -7013,7 +7016,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -7045,7 +7048,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -7077,7 +7080,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -7109,7 +7112,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -7141,7 +7144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -7173,7 +7176,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -7205,7 +7208,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -7237,7 +7240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -7269,7 +7272,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -7301,7 +7304,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -7333,7 +7336,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -7365,7 +7368,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -7397,7 +7400,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -7429,7 +7432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
@@ -7461,7 +7464,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
@@ -7493,7 +7496,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
@@ -7525,7 +7528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
@@ -7557,7 +7560,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
@@ -7589,7 +7592,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
@@ -7621,7 +7624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
@@ -7653,7 +7656,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
@@ -7685,7 +7688,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
@@ -7717,7 +7720,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
@@ -7749,7 +7752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
@@ -7781,7 +7784,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
@@ -7813,7 +7816,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
@@ -7845,7 +7848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
@@ -7877,7 +7880,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
@@ -7909,7 +7912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
@@ -7941,7 +7944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
@@ -7973,7 +7976,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
@@ -8005,7 +8008,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
@@ -8037,7 +8040,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41</v>
       </c>
@@ -8069,7 +8072,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>42</v>
       </c>
@@ -8101,7 +8104,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
@@ -8133,7 +8136,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>44</v>
       </c>
@@ -8165,7 +8168,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
@@ -8197,7 +8200,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
@@ -8229,7 +8232,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
@@ -8261,7 +8264,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
       </c>
@@ -8293,7 +8296,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
@@ -8325,7 +8328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
@@ -8357,7 +8360,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
       </c>
@@ -8389,7 +8392,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
@@ -8421,7 +8424,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
@@ -8453,7 +8456,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>54</v>
       </c>
@@ -8485,7 +8488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
@@ -8517,7 +8520,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>56</v>
       </c>
@@ -8549,7 +8552,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>57</v>
       </c>
@@ -8581,7 +8584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>58</v>
       </c>
@@ -8613,7 +8616,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>59</v>
       </c>
@@ -8645,7 +8648,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>60</v>
       </c>
@@ -8677,7 +8680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>61</v>
       </c>
@@ -8709,7 +8712,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>62</v>
       </c>
@@ -8741,7 +8744,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>63</v>
       </c>
@@ -8773,7 +8776,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>64</v>
       </c>
@@ -8805,7 +8808,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>65</v>
       </c>
@@ -8847,14 +8850,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8">
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>53</v>
       </c>
@@ -8875,7 +8878,7 @@
         <v>username,firstname,lastname,email,auth</v>
       </c>
     </row>
-    <row r="2" spans="3:8" ht="15.75">
+    <row r="2" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C2" s="11">
         <v>15419141</v>
       </c>
@@ -8896,7 +8899,7 @@
         <v>15419141,VEGA CANALES,FELIPE,fvega@undc.edu.pe,oauth2</v>
       </c>
     </row>
-    <row r="3" spans="3:8">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" s="12">
         <v>40662095</v>
       </c>
@@ -8917,7 +8920,7 @@
         <v>40662095,TORRES JIMÉNEZ,EDERSON IGNACIO,e_torres@undc.edu.pe,oauth2</v>
       </c>
     </row>
-    <row r="4" spans="3:8">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="12">
         <v>46117029</v>
       </c>
@@ -8938,7 +8941,7 @@
         <v>46117029,ANTONIO AQUIJE,RENZO ROLAND,rantonio@undc.edu.pe,oauth2</v>
       </c>
     </row>
-    <row r="5" spans="3:8">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="12">
         <v>45976158</v>
       </c>
@@ -8959,7 +8962,7 @@
         <v>45976158,TOLEDO GUERRA,JUAN CARLOS ALFREDO,jtoledo@undc.edu.pe,oauth2</v>
       </c>
     </row>
-    <row r="6" spans="3:8">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="12">
         <v>40332859</v>
       </c>
@@ -8980,7 +8983,7 @@
         <v>40332859,ÑAÑEZ JAVIER,NANCY,nnanez@undc.edu.pe,oauth2</v>
       </c>
     </row>
-    <row r="7" spans="3:8">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="12" t="s">
         <v>36</v>
       </c>
@@ -9001,7 +9004,7 @@
         <v>06532908,VALDERRAMA ROMERO,ANTONIO SALOMON,avalderrama@undc.edu.pe,oauth2</v>
       </c>
     </row>
-    <row r="8" spans="3:8">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="12" t="s">
         <v>38</v>
       </c>
@@ -9036,9 +9039,9 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>155</v>
       </c>
@@ -9046,7 +9049,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -9054,7 +9057,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -9063,7 +9066,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -9072,7 +9075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -9081,7 +9084,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -9090,7 +9093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -9099,7 +9102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>113</v>
       </c>
@@ -9108,7 +9111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -9117,7 +9120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>159</v>
       </c>
@@ -9126,7 +9129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -9135,7 +9138,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>160</v>
       </c>
@@ -9144,7 +9147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14">
         <f>SUM(B4:B13)</f>
         <v>69</v>

</xml_diff>